<commit_message>
minor changes for location
</commit_message>
<xml_diff>
--- a/aerosports/src/assets/data/menu.xlsx
+++ b/aerosports/src/assets/data/menu.xlsx
@@ -1262,7 +1262,7 @@
                     &lt;li&gt;1 FREE Water Bottle Per Visit&lt;/li&gt;
                     &lt;li&gt;25% OFF Sibling Membership&lt;/li&gt;
                 &lt;/ul&gt;
-                &lt;p&gt;Monthly Payment: $9.90&lt;/p&gt;
+                &lt;p&gt;Monthly Payment: $9.90&lt;/p&gt;&lt;h4&gt;OR&lt;/h4&gt;
                 &lt;p&gt;Annual Payment: $99.90&lt;/p&gt;
             &lt;/div&gt;
             &lt;div class="membership-membership-platinum"&gt;
@@ -1270,7 +1270,7 @@
                 &lt;h2 class="membership-container-heading"&gt;Platinum Member Perks!&lt;/h2&gt;
                 &lt;ul class="membership-list"&gt;
                     &lt;li&gt;First Jump FREE&lt;/li&gt;
-                    &lt;li&gt;Cash Discount of $150 OFF a&lt;/li&gt;
+                    &lt;li&gt;Cash Discount of $150 OFF&lt;/li&gt;
                     &lt;li&gt;Birthday Party Booking&lt;/li&gt;
                     &lt;li&gt;$15 OFF Jump Times "&lt;/li&gt;
                     &lt;li&gt;50% OFF Aero Camp&lt;/li&gt;
@@ -1279,9 +1279,9 @@
                     &lt;li&gt;1 FREE Water Bottle Per Visit&lt;/li&gt;
                     &lt;li&gt;25% OFF Sibling Membership&lt;/li&gt;
                 &lt;/ul&gt;
-                &lt;p&gt;Monthly Payment: $14.90&lt;/p&gt;
+                &lt;p&gt;Monthly Payment: $14.90&lt;/p&gt;&lt;h4&gt;OR&lt;/h4&gt;
                 &lt;p&gt;Annual Payment: $140&lt;/p&gt;
-            &lt;/div&gt; &lt;div class="col section-button  text-center"&gt;&lt;a class="sigma_btn-custom" href="https://ecom.roller.app/aerosportslondon/londoncheckout/en/home?utm_source=brevo&amp;amp;utm_campaign=Memberships are Here&amp;amp;utm_medium=email" target="_blank" data-btn="1" style="font-style: normal; font-weight: bold; line-height: 1.15; text-decoration: none; word-break: break-word; border-style: solid; word-wrap: break-word; display: block; -webkit-text-size-adjust: none; background-color: #051ef4; border-color: #051ef4; border-radius: 20px; border-width: 0px; color: #ffffff; font-family: arial,helvetica,sans-serif; font-size: 16px; height: 18px; mso-hide: all; padding-bottom: 12px; padding-top: 12px; width: 205px;"&gt; &lt;span&gt;SIGN UP NOW&lt;/span&gt;&lt;/a&gt;&lt;/div&gt;
+            &lt;/div&gt; &lt;div class="col section-button  text-center"&gt;&lt;a id="signup-button" class="sigma_btn-custom" href="https://ecom.roller.app/aerosports{location.url}/memberships/en/home" target="_blank" data-btn="1" style="font-style: normal; font-weight: bold; line-height: 1.15; text-decoration: none; word-break: break-word; border-style: solid; word-wrap: break-word; display: block; -webkit-text-size-adjust: none; background-color: #051ef4; border-color: #051ef4; border-radius: 20px; border-width: 0px; color: #ffffff; font-family: arial,helvetica,sans-serif; font-size: 16px; height: 18px; mso-hide: all; padding-bottom: 12px; padding-top: 12px; width: 205px;"&gt; &lt;span&gt;SIGN UP NOW&lt;/span&gt;&lt;/a&gt;&lt;/div&gt;
         &lt;/div&gt;
     &lt;/div&gt;
 &lt;/body&gt;
@@ -11210,7 +11210,7 @@
       <c r="B61" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="2" t="s">
         <v>438</v>
       </c>
     </row>
@@ -11221,7 +11221,7 @@
       <c r="B62" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="2" t="s">
         <v>439</v>
       </c>
     </row>
@@ -13354,7 +13354,7 @@
       <c r="D2" s="1">
         <v>350.0</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="2" t="s">
         <v>461</v>
       </c>
     </row>
@@ -13388,7 +13388,7 @@
       <c r="D4" s="1">
         <v>650.0</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="2" t="s">
         <v>466</v>
       </c>
     </row>
@@ -13422,7 +13422,7 @@
       <c r="D6" s="1">
         <v>325.0</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="2" t="s">
         <v>469</v>
       </c>
     </row>
@@ -13439,7 +13439,7 @@
       <c r="D7" s="1">
         <v>600.0</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="2" t="s">
         <v>470</v>
       </c>
     </row>
@@ -13456,7 +13456,7 @@
       <c r="D8" s="1">
         <v>300.0</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="2" t="s">
         <v>471</v>
       </c>
     </row>
@@ -13473,7 +13473,7 @@
       <c r="D9" s="1">
         <v>560.0</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="2" t="s">
         <v>472</v>
       </c>
     </row>
@@ -13490,7 +13490,7 @@
       <c r="D10" s="1">
         <v>400.0</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="2" t="s">
         <v>473</v>
       </c>
     </row>
@@ -13507,7 +13507,7 @@
       <c r="D11" s="1">
         <v>300.0</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="2" t="s">
         <v>475</v>
       </c>
     </row>
@@ -13524,7 +13524,7 @@
       <c r="D12" s="1">
         <v>560.0</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="2" t="s">
         <v>476</v>
       </c>
     </row>
@@ -13541,7 +13541,7 @@
       <c r="D13" s="1">
         <v>400.0</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="2" t="s">
         <v>477</v>
       </c>
     </row>
@@ -13558,7 +13558,7 @@
       <c r="D14" s="1">
         <v>240.0</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="2" t="s">
         <v>479</v>
       </c>
     </row>
@@ -13575,7 +13575,7 @@
       <c r="D15" s="1">
         <v>240.0</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="2" t="s">
         <v>481</v>
       </c>
     </row>

</xml_diff>